<commit_message>
Adding linear regression in Excel file example
</commit_message>
<xml_diff>
--- a/assets/scripts/MetLife_1999_ideal_body_weight_table.xlsx
+++ b/assets/scripts/MetLife_1999_ideal_body_weight_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PSL/Dropbox/Work/Médecine/Internat/Data Sci geekeries PAR/linear regression/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PSL/Desktop/tomboulier.github.io/assets/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB76722C-E3AE-4D4A-88BF-1EE8AA87CDC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9048AAF-0B47-7149-9665-B491CA8A4CCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15460" xr2:uid="{AC078919-1348-F741-AFBE-5AA9DDE5FCBB}"/>
   </bookViews>
@@ -241,6 +241,22 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Feuil1!$E$3:$E$17</c:f>
@@ -1559,7 +1575,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>